<commit_message>
prep for study 3: adults and hierarchical jobs
</commit_message>
<xml_diff>
--- a/data/strConseq_data_pilot2.xlsx
+++ b/data/strConseq_data_pilot2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Stanford\projects\structural-consequences\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8520CA-B73F-4F55-B19D-9C30488CBA71}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F98FAD9-CA6C-4079-BACD-5797CD854084}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2100" yWindow="210" windowWidth="18410" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="178">
   <si>
     <t>consent</t>
   </si>
@@ -560,6 +560,12 @@
   </si>
   <si>
     <t>normativity_fc</t>
+  </si>
+  <si>
+    <t>check_group_berry_coded</t>
+  </si>
+  <si>
+    <t>chromebook</t>
   </si>
 </sst>
 </file>
@@ -1611,10 +1617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AQ154"/>
+  <dimension ref="A1:AR154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AI24" sqref="AI24"/>
+    <sheetView tabSelected="1" topLeftCell="X1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AA11" sqref="AA11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1641,22 +1647,23 @@
     <col min="23" max="23" width="15.81640625" customWidth="1"/>
     <col min="24" max="24" width="16.6328125" style="5" customWidth="1"/>
     <col min="25" max="25" width="18.81640625" style="22" customWidth="1"/>
-    <col min="26" max="26" width="19.08984375" customWidth="1"/>
-    <col min="27" max="27" width="16.54296875" customWidth="1"/>
-    <col min="28" max="30" width="12.6328125" customWidth="1"/>
-    <col min="31" max="31" width="19.1796875" customWidth="1"/>
-    <col min="32" max="32" width="16.1796875" customWidth="1"/>
-    <col min="33" max="33" width="33.453125" customWidth="1"/>
-    <col min="34" max="35" width="18.1796875" customWidth="1"/>
-    <col min="36" max="36" width="16.90625" customWidth="1"/>
-    <col min="37" max="37" width="12.6328125" style="35" customWidth="1"/>
-    <col min="38" max="40" width="12.6328125" style="36" customWidth="1"/>
-    <col min="41" max="41" width="12.6328125" style="37" customWidth="1"/>
-    <col min="42" max="42" width="12.6328125" style="25" customWidth="1"/>
-    <col min="43" max="43" width="17.7265625" customWidth="1"/>
+    <col min="26" max="26" width="18.81640625" customWidth="1"/>
+    <col min="27" max="27" width="19.08984375" customWidth="1"/>
+    <col min="28" max="28" width="16.54296875" customWidth="1"/>
+    <col min="29" max="31" width="12.6328125" customWidth="1"/>
+    <col min="32" max="32" width="19.1796875" customWidth="1"/>
+    <col min="33" max="33" width="16.1796875" customWidth="1"/>
+    <col min="34" max="34" width="33.453125" customWidth="1"/>
+    <col min="35" max="36" width="18.1796875" customWidth="1"/>
+    <col min="37" max="37" width="16.90625" customWidth="1"/>
+    <col min="38" max="38" width="12.6328125" style="35" customWidth="1"/>
+    <col min="39" max="41" width="12.6328125" style="36" customWidth="1"/>
+    <col min="42" max="42" width="12.6328125" style="37" customWidth="1"/>
+    <col min="43" max="43" width="12.6328125" style="25" customWidth="1"/>
+    <col min="44" max="44" width="17.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:44" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>13</v>
       </c>
@@ -1732,62 +1739,65 @@
       <c r="Y1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="Z1" s="10" t="s">
+      <c r="Z1" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="AA1" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="AA1" s="10" t="s">
+      <c r="AB1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="AB1" s="10" t="s">
+      <c r="AC1" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="AC1" s="10" t="s">
+      <c r="AD1" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="AD1" s="10" t="s">
+      <c r="AE1" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="AE1" s="10" t="s">
+      <c r="AF1" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="AF1" s="10" t="s">
+      <c r="AG1" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="AG1" s="10" t="s">
+      <c r="AH1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="AH1" s="10" t="s">
+      <c r="AI1" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="AI1" s="10" t="s">
+      <c r="AJ1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="AJ1" s="10" t="s">
+      <c r="AK1" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="AK1" s="32" t="s">
+      <c r="AL1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="AL1" s="33" t="s">
+      <c r="AM1" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="AM1" s="33" t="s">
+      <c r="AN1" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="AN1" s="33" t="s">
+      <c r="AO1" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="AO1" s="34" t="s">
+      <c r="AP1" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="AP1" s="24" t="s">
+      <c r="AQ1" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="AQ1" s="10" t="s">
+      <c r="AR1" s="10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>54</v>
       </c>
@@ -1864,56 +1874,60 @@
       <c r="Y2" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="Z2" t="s">
-        <v>59</v>
+      <c r="Z2" s="1">
+        <f>IF(N2="ZarpiesVawns", IF(Y2="Vawns", 1, 0), IF(Y2="Zarpies", 1, 0))</f>
+        <v>1</v>
       </c>
       <c r="AA2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB2" t="s">
         <v>62</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>60</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>63</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>64</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
         <v>65</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AH2" t="s">
         <v>123</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AI2" t="s">
         <v>132</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AJ2" t="s">
         <v>66</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AK2" t="s">
         <v>124</v>
       </c>
-      <c r="AK2" s="35">
+      <c r="AL2" s="35">
         <v>3</v>
       </c>
-      <c r="AL2" s="36" t="s">
+      <c r="AM2" s="36" t="s">
         <v>58</v>
-      </c>
-      <c r="AM2" s="36">
-        <v>5</v>
       </c>
       <c r="AN2" s="36">
         <v>5</v>
       </c>
-      <c r="AO2" s="37">
+      <c r="AO2" s="36">
         <v>5</v>
       </c>
-      <c r="AP2" s="25" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.35">
+      <c r="AP2" s="37">
+        <v>5</v>
+      </c>
+      <c r="AQ2" s="25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>77</v>
       </c>
@@ -1990,56 +2004,60 @@
       <c r="Y3" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="Z3" t="s">
-        <v>59</v>
+      <c r="Z3" s="1">
+        <f t="shared" ref="Z3:Z24" si="1">IF(N3="ZarpiesVawns", IF(Y3="Vawns", 1, 0), IF(Y3="Zarpies", 1, 0))</f>
+        <v>1</v>
       </c>
       <c r="AA3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB3" t="s">
         <v>62</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AD3" t="s">
         <v>60</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AE3" t="s">
         <v>63</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AF3" t="s">
         <v>64</v>
       </c>
-      <c r="AF3" t="s">
+      <c r="AG3" t="s">
         <v>65</v>
       </c>
-      <c r="AG3" t="s">
+      <c r="AH3" t="s">
         <v>125</v>
       </c>
-      <c r="AH3" t="s">
+      <c r="AI3" t="s">
         <v>132</v>
       </c>
-      <c r="AI3" t="s">
+      <c r="AJ3" t="s">
         <v>76</v>
       </c>
-      <c r="AJ3" t="s">
+      <c r="AK3" t="s">
         <v>126</v>
       </c>
-      <c r="AK3" s="35">
-        <v>1</v>
-      </c>
-      <c r="AL3" s="36" t="s">
+      <c r="AL3" s="35">
+        <v>1</v>
+      </c>
+      <c r="AM3" s="36" t="s">
         <v>75</v>
-      </c>
-      <c r="AM3" s="36">
-        <v>4</v>
       </c>
       <c r="AN3" s="36">
         <v>4</v>
       </c>
-      <c r="AO3" s="37">
+      <c r="AO3" s="36">
         <v>4</v>
       </c>
-      <c r="AP3" s="25" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.35">
+      <c r="AP3" s="37">
+        <v>4</v>
+      </c>
+      <c r="AQ3" s="25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>78</v>
       </c>
@@ -2116,53 +2134,57 @@
       <c r="Y4" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="Z4" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AA4" t="s">
         <v>57</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AB4" t="s">
         <v>81</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AD4" t="s">
         <v>67</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="AE4" t="s">
         <v>82</v>
       </c>
-      <c r="AE4" t="s">
+      <c r="AF4" t="s">
         <v>83</v>
       </c>
-      <c r="AF4" t="s">
+      <c r="AG4" t="s">
         <v>84</v>
       </c>
-      <c r="AG4" t="s">
+      <c r="AH4" t="s">
         <v>127</v>
       </c>
-      <c r="AH4" t="s">
+      <c r="AI4" t="s">
         <v>151</v>
       </c>
-      <c r="AI4" t="s">
+      <c r="AJ4" t="s">
         <v>85</v>
       </c>
-      <c r="AK4" s="35">
+      <c r="AL4" s="35">
         <v>2</v>
       </c>
-      <c r="AL4" s="36" t="s">
+      <c r="AM4" s="36" t="s">
         <v>80</v>
-      </c>
-      <c r="AM4" s="36">
-        <v>5</v>
       </c>
       <c r="AN4" s="36">
         <v>5</v>
       </c>
-      <c r="AO4" s="37">
+      <c r="AO4" s="36">
         <v>5</v>
       </c>
-      <c r="AP4" s="25" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.35">
+      <c r="AP4" s="37">
+        <v>5</v>
+      </c>
+      <c r="AQ4" s="25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>94</v>
       </c>
@@ -2237,55 +2259,59 @@
         <v>67</v>
       </c>
       <c r="Y5" s="23" t="s">
-        <v>96</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>59</v>
+        <v>61</v>
+      </c>
+      <c r="Z5" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="AA5" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB5" t="s">
         <v>62</v>
       </c>
-      <c r="AC5" t="s">
+      <c r="AD5" t="s">
         <v>67</v>
       </c>
-      <c r="AD5" t="s">
+      <c r="AE5" t="s">
         <v>97</v>
       </c>
-      <c r="AE5" t="s">
+      <c r="AF5" t="s">
         <v>83</v>
       </c>
-      <c r="AF5" t="s">
+      <c r="AG5" t="s">
         <v>84</v>
       </c>
-      <c r="AG5" t="s">
+      <c r="AH5" t="s">
         <v>128</v>
       </c>
-      <c r="AH5" t="s">
+      <c r="AI5" t="s">
         <v>133</v>
       </c>
-      <c r="AI5" t="s">
+      <c r="AJ5" t="s">
         <v>98</v>
       </c>
-      <c r="AK5" s="35">
-        <v>1</v>
-      </c>
-      <c r="AL5" s="36" t="s">
+      <c r="AL5" s="35">
+        <v>1</v>
+      </c>
+      <c r="AM5" s="36" t="s">
         <v>95</v>
-      </c>
-      <c r="AM5" s="36">
-        <v>5</v>
       </c>
       <c r="AN5" s="36">
         <v>5</v>
       </c>
-      <c r="AO5" s="37">
+      <c r="AO5" s="36">
         <v>5</v>
       </c>
-      <c r="AP5" s="25" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.35">
+      <c r="AP5" s="37">
+        <v>5</v>
+      </c>
+      <c r="AQ5" s="25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>99</v>
       </c>
@@ -2362,50 +2388,54 @@
       <c r="Y6" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="Z6" t="s">
-        <v>59</v>
+      <c r="Z6" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="AA6" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB6" t="s">
         <v>62</v>
       </c>
-      <c r="AC6" t="s">
+      <c r="AD6" t="s">
         <v>60</v>
       </c>
-      <c r="AD6" t="s">
+      <c r="AE6" t="s">
         <v>63</v>
       </c>
-      <c r="AE6" t="s">
+      <c r="AF6" t="s">
         <v>64</v>
       </c>
-      <c r="AF6" t="s">
+      <c r="AG6" t="s">
         <v>65</v>
       </c>
-      <c r="AG6" t="s">
+      <c r="AH6" t="s">
         <v>101</v>
       </c>
-      <c r="AH6" t="s">
+      <c r="AI6" t="s">
         <v>139</v>
       </c>
-      <c r="AK6" s="35">
+      <c r="AL6" s="35">
         <v>2</v>
       </c>
-      <c r="AL6" s="36" t="s">
+      <c r="AM6" s="36" t="s">
         <v>100</v>
-      </c>
-      <c r="AM6" s="36">
-        <v>5</v>
       </c>
       <c r="AN6" s="36">
         <v>5</v>
       </c>
-      <c r="AO6" s="37">
+      <c r="AO6" s="36">
+        <v>5</v>
+      </c>
+      <c r="AP6" s="37">
         <v>3</v>
       </c>
-      <c r="AP6" s="25" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.35">
+      <c r="AQ6" s="25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>102</v>
       </c>
@@ -2480,55 +2510,59 @@
         <v>67</v>
       </c>
       <c r="Y7" s="23" t="s">
-        <v>96</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>59</v>
+        <v>61</v>
+      </c>
+      <c r="Z7" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="AA7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB7" t="s">
         <v>62</v>
       </c>
-      <c r="AC7" t="s">
+      <c r="AD7" t="s">
         <v>60</v>
       </c>
-      <c r="AD7" t="s">
+      <c r="AE7" t="s">
         <v>104</v>
       </c>
-      <c r="AE7" t="s">
+      <c r="AF7" t="s">
         <v>64</v>
       </c>
-      <c r="AF7" t="s">
+      <c r="AG7" t="s">
         <v>105</v>
       </c>
-      <c r="AG7" t="s">
+      <c r="AH7" t="s">
         <v>129</v>
       </c>
-      <c r="AH7" t="s">
+      <c r="AI7" t="s">
         <v>132</v>
       </c>
-      <c r="AI7" t="s">
+      <c r="AJ7" t="s">
         <v>98</v>
       </c>
-      <c r="AK7" s="35">
-        <v>1</v>
-      </c>
-      <c r="AL7" s="36" t="s">
+      <c r="AL7" s="35">
+        <v>1</v>
+      </c>
+      <c r="AM7" s="36" t="s">
         <v>103</v>
-      </c>
-      <c r="AM7" s="36">
-        <v>5</v>
       </c>
       <c r="AN7" s="36">
         <v>5</v>
       </c>
-      <c r="AO7" s="37">
+      <c r="AO7" s="36">
         <v>5</v>
       </c>
-      <c r="AP7" s="25" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.35">
+      <c r="AP7" s="37">
+        <v>5</v>
+      </c>
+      <c r="AQ7" s="25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>106</v>
       </c>
@@ -2605,56 +2639,63 @@
       <c r="Y8" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="Z8" t="s">
-        <v>59</v>
+      <c r="Z8" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="AA8" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB8" t="s">
         <v>62</v>
       </c>
-      <c r="AC8" t="s">
+      <c r="AD8" t="s">
         <v>60</v>
       </c>
-      <c r="AD8" t="s">
+      <c r="AE8" t="s">
         <v>63</v>
       </c>
-      <c r="AE8" t="s">
+      <c r="AF8" t="s">
         <v>83</v>
       </c>
-      <c r="AF8" t="s">
+      <c r="AG8" t="s">
         <v>84</v>
       </c>
-      <c r="AG8" t="s">
+      <c r="AH8" t="s">
         <v>130</v>
       </c>
-      <c r="AH8" t="s">
+      <c r="AI8" t="s">
         <v>151</v>
       </c>
-      <c r="AI8" t="s">
+      <c r="AJ8" t="s">
         <v>107</v>
       </c>
-      <c r="AJ8" t="s">
+      <c r="AK8" t="s">
         <v>108</v>
       </c>
-      <c r="AK8" s="35">
+      <c r="AL8" s="35">
         <v>2</v>
       </c>
-      <c r="AM8" s="36">
+      <c r="AM8" s="36" t="s">
+        <v>177</v>
+      </c>
+      <c r="AN8" s="36">
         <v>4</v>
       </c>
-      <c r="AN8" s="36">
+      <c r="AO8" s="36">
         <v>5</v>
       </c>
-      <c r="AO8" s="37">
+      <c r="AP8" s="37">
         <v>5</v>
       </c>
-      <c r="AP8" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="AQ8" t="s">
+      <c r="AQ8" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="AR8" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>110</v>
       </c>
@@ -2729,55 +2770,59 @@
         <v>67</v>
       </c>
       <c r="Y9" s="23" t="s">
-        <v>96</v>
-      </c>
-      <c r="Z9" t="s">
-        <v>59</v>
+        <v>61</v>
+      </c>
+      <c r="Z9" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="AA9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB9" t="s">
         <v>62</v>
       </c>
-      <c r="AC9" t="s">
+      <c r="AD9" t="s">
         <v>60</v>
       </c>
-      <c r="AD9" t="s">
+      <c r="AE9" t="s">
         <v>63</v>
       </c>
-      <c r="AE9" t="s">
+      <c r="AF9" t="s">
         <v>83</v>
       </c>
-      <c r="AF9" t="s">
+      <c r="AG9" t="s">
         <v>112</v>
       </c>
-      <c r="AG9" t="s">
+      <c r="AH9" t="s">
         <v>136</v>
       </c>
-      <c r="AH9" t="s">
+      <c r="AI9" t="s">
         <v>134</v>
       </c>
-      <c r="AI9" t="s">
+      <c r="AJ9" t="s">
         <v>66</v>
       </c>
-      <c r="AK9" s="35">
+      <c r="AL9" s="35">
         <v>3</v>
       </c>
-      <c r="AL9" s="36" t="s">
+      <c r="AM9" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="AM9" s="36">
+      <c r="AN9" s="36">
         <v>5</v>
       </c>
-      <c r="AN9" s="36">
-        <v>1</v>
-      </c>
-      <c r="AO9" s="37">
+      <c r="AO9" s="36">
+        <v>1</v>
+      </c>
+      <c r="AP9" s="37">
         <v>5</v>
       </c>
-      <c r="AP9" s="25" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.35">
+      <c r="AQ9" s="25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>114</v>
       </c>
@@ -2852,55 +2897,59 @@
         <v>67</v>
       </c>
       <c r="Y10" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="Z10" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z10" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AA10" t="s">
         <v>57</v>
       </c>
-      <c r="AA10" t="s">
+      <c r="AB10" t="s">
         <v>81</v>
       </c>
-      <c r="AC10" t="s">
+      <c r="AD10" t="s">
         <v>67</v>
       </c>
-      <c r="AD10" t="s">
+      <c r="AE10" t="s">
         <v>82</v>
       </c>
-      <c r="AE10" t="s">
+      <c r="AF10" t="s">
         <v>83</v>
       </c>
-      <c r="AF10" t="s">
+      <c r="AG10" t="s">
         <v>84</v>
       </c>
-      <c r="AG10" t="s">
+      <c r="AH10" t="s">
         <v>137</v>
       </c>
-      <c r="AH10" t="s">
+      <c r="AI10" t="s">
         <v>151</v>
       </c>
-      <c r="AI10" t="s">
+      <c r="AJ10" t="s">
         <v>66</v>
       </c>
-      <c r="AK10" s="35">
+      <c r="AL10" s="35">
         <v>2</v>
       </c>
-      <c r="AL10" s="36" t="s">
+      <c r="AM10" s="36" t="s">
         <v>115</v>
-      </c>
-      <c r="AM10" s="36">
-        <v>5</v>
       </c>
       <c r="AN10" s="36">
         <v>5</v>
       </c>
-      <c r="AO10" s="37">
+      <c r="AO10" s="36">
         <v>5</v>
       </c>
-      <c r="AP10" s="25" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.35">
+      <c r="AP10" s="37">
+        <v>5</v>
+      </c>
+      <c r="AQ10" s="25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>118</v>
       </c>
@@ -2975,55 +3024,59 @@
         <v>67</v>
       </c>
       <c r="Y11" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="Z11" t="s">
-        <v>59</v>
+        <v>96</v>
+      </c>
+      <c r="Z11" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="AA11" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB11" t="s">
         <v>62</v>
       </c>
-      <c r="AC11" t="s">
+      <c r="AD11" t="s">
         <v>60</v>
       </c>
-      <c r="AD11" t="s">
+      <c r="AE11" t="s">
         <v>63</v>
       </c>
-      <c r="AE11" t="s">
+      <c r="AF11" t="s">
         <v>83</v>
       </c>
-      <c r="AF11" t="s">
+      <c r="AG11" t="s">
         <v>84</v>
       </c>
-      <c r="AG11" t="s">
+      <c r="AH11" t="s">
         <v>138</v>
       </c>
-      <c r="AH11" t="s">
+      <c r="AI11" t="s">
         <v>151</v>
       </c>
-      <c r="AI11" t="s">
+      <c r="AJ11" t="s">
         <v>66</v>
       </c>
-      <c r="AK11" s="35">
+      <c r="AL11" s="35">
         <v>2</v>
       </c>
-      <c r="AL11" s="36" t="s">
+      <c r="AM11" s="36" t="s">
         <v>119</v>
-      </c>
-      <c r="AM11" s="36">
-        <v>5</v>
       </c>
       <c r="AN11" s="36">
         <v>5</v>
       </c>
-      <c r="AO11" s="37">
+      <c r="AO11" s="36">
         <v>5</v>
       </c>
-      <c r="AP11" s="25" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.35">
+      <c r="AP11" s="37">
+        <v>5</v>
+      </c>
+      <c r="AQ11" s="25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>120</v>
       </c>
@@ -3098,55 +3151,59 @@
         <v>67</v>
       </c>
       <c r="Y12" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="Z12" t="s">
-        <v>59</v>
+        <v>96</v>
+      </c>
+      <c r="Z12" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="AA12" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB12" t="s">
         <v>62</v>
       </c>
-      <c r="AC12" t="s">
+      <c r="AD12" t="s">
         <v>60</v>
       </c>
-      <c r="AD12" t="s">
+      <c r="AE12" t="s">
         <v>104</v>
       </c>
-      <c r="AE12" t="s">
+      <c r="AF12" t="s">
         <v>83</v>
       </c>
-      <c r="AF12" t="s">
+      <c r="AG12" t="s">
         <v>112</v>
       </c>
-      <c r="AG12" t="s">
+      <c r="AH12" t="s">
         <v>122</v>
       </c>
-      <c r="AH12" t="s">
+      <c r="AI12" t="s">
         <v>135</v>
       </c>
-      <c r="AI12" t="s">
+      <c r="AJ12" t="s">
         <v>66</v>
       </c>
-      <c r="AK12" s="35">
+      <c r="AL12" s="35">
         <v>2</v>
       </c>
-      <c r="AL12" s="36" t="s">
+      <c r="AM12" s="36" t="s">
         <v>100</v>
-      </c>
-      <c r="AM12" s="36">
-        <v>5</v>
       </c>
       <c r="AN12" s="36">
         <v>5</v>
       </c>
-      <c r="AO12" s="37">
+      <c r="AO12" s="36">
+        <v>5</v>
+      </c>
+      <c r="AP12" s="37">
         <v>4</v>
       </c>
-      <c r="AP12" s="25" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.35">
+      <c r="AQ12" s="25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>140</v>
       </c>
@@ -3223,56 +3280,60 @@
       <c r="Y13" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="Z13" t="s">
-        <v>59</v>
+      <c r="Z13" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="AA13" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB13" t="s">
         <v>62</v>
       </c>
-      <c r="AC13" t="s">
+      <c r="AD13" t="s">
         <v>60</v>
       </c>
-      <c r="AD13" t="s">
+      <c r="AE13" t="s">
         <v>63</v>
       </c>
-      <c r="AE13" t="s">
+      <c r="AF13" t="s">
         <v>64</v>
       </c>
-      <c r="AF13" t="s">
+      <c r="AG13" t="s">
         <v>105</v>
       </c>
-      <c r="AG13" t="s">
+      <c r="AH13" t="s">
         <v>141</v>
       </c>
-      <c r="AH13" t="s">
+      <c r="AI13" t="s">
         <v>151</v>
       </c>
-      <c r="AI13" t="s">
+      <c r="AJ13" t="s">
         <v>98</v>
       </c>
-      <c r="AJ13" t="s">
+      <c r="AK13" t="s">
         <v>142</v>
       </c>
-      <c r="AK13" s="35">
-        <v>1</v>
-      </c>
-      <c r="AL13" s="36" t="s">
+      <c r="AL13" s="35">
+        <v>1</v>
+      </c>
+      <c r="AM13" s="36" t="s">
         <v>143</v>
-      </c>
-      <c r="AM13" s="36">
-        <v>5</v>
       </c>
       <c r="AN13" s="36">
         <v>5</v>
       </c>
-      <c r="AO13" s="37">
+      <c r="AO13" s="36">
         <v>5</v>
       </c>
-      <c r="AP13" s="25" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="14" spans="1:43" x14ac:dyDescent="0.35">
+      <c r="AP13" s="37">
+        <v>5</v>
+      </c>
+      <c r="AQ13" s="25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>145</v>
       </c>
@@ -3349,53 +3410,57 @@
       <c r="Y14" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="Z14" t="s">
-        <v>59</v>
+      <c r="Z14" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="AA14" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB14" t="s">
         <v>62</v>
       </c>
-      <c r="AC14" t="s">
+      <c r="AD14" t="s">
         <v>60</v>
       </c>
-      <c r="AD14" t="s">
+      <c r="AE14" t="s">
         <v>104</v>
       </c>
-      <c r="AE14" t="s">
+      <c r="AF14" t="s">
         <v>83</v>
       </c>
-      <c r="AF14" t="s">
+      <c r="AG14" t="s">
         <v>112</v>
       </c>
-      <c r="AG14" t="s">
+      <c r="AH14" t="s">
         <v>147</v>
       </c>
-      <c r="AH14" t="s">
+      <c r="AI14" t="s">
         <v>134</v>
       </c>
-      <c r="AI14" t="s">
+      <c r="AJ14" t="s">
         <v>66</v>
       </c>
-      <c r="AK14" s="35">
+      <c r="AL14" s="35">
         <v>3</v>
       </c>
-      <c r="AL14" s="36" t="s">
+      <c r="AM14" s="36" t="s">
         <v>146</v>
       </c>
-      <c r="AM14" s="36">
+      <c r="AN14" s="36">
         <v>4</v>
       </c>
-      <c r="AN14" s="36">
+      <c r="AO14" s="36">
         <v>5</v>
       </c>
-      <c r="AO14" s="37">
+      <c r="AP14" s="37">
         <v>4</v>
       </c>
-      <c r="AP14" s="25" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.35">
+      <c r="AQ14" s="25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>148</v>
       </c>
@@ -3472,53 +3537,57 @@
       <c r="Y15" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="Z15" t="s">
+      <c r="Z15" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AA15" t="s">
         <v>57</v>
       </c>
-      <c r="AA15" t="s">
+      <c r="AB15" t="s">
         <v>81</v>
       </c>
-      <c r="AC15" t="s">
+      <c r="AD15" t="s">
         <v>67</v>
       </c>
-      <c r="AD15" t="s">
+      <c r="AE15" t="s">
         <v>82</v>
       </c>
-      <c r="AE15" t="s">
+      <c r="AF15" t="s">
         <v>83</v>
       </c>
-      <c r="AF15" t="s">
+      <c r="AG15" t="s">
         <v>112</v>
       </c>
-      <c r="AG15" t="s">
+      <c r="AH15" t="s">
         <v>150</v>
       </c>
-      <c r="AH15" t="s">
+      <c r="AI15" t="s">
         <v>151</v>
       </c>
-      <c r="AI15" t="s">
+      <c r="AJ15" t="s">
         <v>66</v>
       </c>
-      <c r="AK15" s="35">
+      <c r="AL15" s="35">
         <v>2</v>
       </c>
-      <c r="AL15" s="36" t="s">
+      <c r="AM15" s="36" t="s">
         <v>149</v>
-      </c>
-      <c r="AM15" s="36">
-        <v>5</v>
       </c>
       <c r="AN15" s="36">
         <v>5</v>
       </c>
-      <c r="AO15" s="37">
+      <c r="AO15" s="36">
+        <v>5</v>
+      </c>
+      <c r="AP15" s="37">
         <v>3</v>
       </c>
-      <c r="AP15" s="25" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:43" x14ac:dyDescent="0.35">
+      <c r="AQ15" s="25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>154</v>
       </c>
@@ -3565,7 +3634,7 @@
         <v>49</v>
       </c>
       <c r="P16" s="4" t="str">
-        <f t="shared" ref="P16" si="1">IF(COUNTIF(Q16:T16,"yes")&gt;0,"yes",IF(COUNTBLANK(Q16:T16)&gt;0,"","no"))</f>
+        <f t="shared" ref="P16" si="2">IF(COUNTIF(Q16:T16,"yes")&gt;0,"yes",IF(COUNTBLANK(Q16:T16)&gt;0,"","no"))</f>
         <v>no</v>
       </c>
       <c r="Q16" s="6" t="s">
@@ -3593,61 +3662,65 @@
         <v>67</v>
       </c>
       <c r="Y16" s="23" t="s">
-        <v>96</v>
-      </c>
-      <c r="Z16" t="s">
-        <v>59</v>
+        <v>61</v>
+      </c>
+      <c r="Z16" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="AA16" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB16" t="s">
         <v>156</v>
       </c>
-      <c r="AC16" t="s">
+      <c r="AD16" t="s">
         <v>67</v>
       </c>
-      <c r="AD16" t="s">
+      <c r="AE16" t="s">
         <v>82</v>
       </c>
-      <c r="AE16" t="s">
+      <c r="AF16" t="s">
         <v>83</v>
       </c>
-      <c r="AF16" t="s">
+      <c r="AG16" t="s">
         <v>84</v>
       </c>
-      <c r="AG16" t="s">
+      <c r="AH16" t="s">
         <v>157</v>
       </c>
-      <c r="AH16" t="s">
+      <c r="AI16" t="s">
         <v>151</v>
       </c>
-      <c r="AI16" t="s">
+      <c r="AJ16" t="s">
         <v>76</v>
       </c>
-      <c r="AJ16" t="s">
+      <c r="AK16" t="s">
         <v>158</v>
       </c>
-      <c r="AK16" s="35">
+      <c r="AL16" s="35">
         <v>2</v>
       </c>
-      <c r="AL16" s="36" t="s">
+      <c r="AM16" s="36" t="s">
         <v>155</v>
       </c>
-      <c r="AM16" s="36">
+      <c r="AN16" s="36">
         <v>3</v>
       </c>
-      <c r="AN16" s="36">
+      <c r="AO16" s="36">
         <v>5</v>
       </c>
-      <c r="AO16" s="37">
+      <c r="AP16" s="37">
         <v>3</v>
       </c>
-      <c r="AP16" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="AQ16" t="s">
+      <c r="AQ16" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="AR16" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="17" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>160</v>
       </c>
@@ -3694,7 +3767,7 @@
         <v>49</v>
       </c>
       <c r="P17" s="4" t="str">
-        <f t="shared" ref="P17" si="2">IF(COUNTIF(Q17:T17,"yes")&gt;0,"yes",IF(COUNTBLANK(Q17:T17)&gt;0,"","no"))</f>
+        <f t="shared" ref="P17" si="3">IF(COUNTIF(Q17:T17,"yes")&gt;0,"yes",IF(COUNTBLANK(Q17:T17)&gt;0,"","no"))</f>
         <v>no</v>
       </c>
       <c r="Q17" s="6" t="s">
@@ -3722,55 +3795,59 @@
         <v>67</v>
       </c>
       <c r="Y17" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="Z17" t="s">
-        <v>59</v>
+        <v>96</v>
+      </c>
+      <c r="Z17" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="AA17" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB17" t="s">
         <v>62</v>
       </c>
-      <c r="AC17" t="s">
+      <c r="AD17" t="s">
         <v>60</v>
       </c>
-      <c r="AD17" t="s">
+      <c r="AE17" t="s">
         <v>63</v>
       </c>
-      <c r="AE17" t="s">
+      <c r="AF17" t="s">
         <v>83</v>
       </c>
-      <c r="AF17" t="s">
+      <c r="AG17" t="s">
         <v>84</v>
       </c>
-      <c r="AG17" t="s">
+      <c r="AH17" t="s">
         <v>162</v>
       </c>
-      <c r="AH17" t="s">
+      <c r="AI17" t="s">
         <v>132</v>
       </c>
-      <c r="AI17" t="s">
+      <c r="AJ17" t="s">
         <v>76</v>
       </c>
-      <c r="AK17" s="35">
+      <c r="AL17" s="35">
         <v>3</v>
       </c>
-      <c r="AL17" s="36" t="s">
+      <c r="AM17" s="36" t="s">
         <v>161</v>
-      </c>
-      <c r="AM17" s="36">
-        <v>5</v>
       </c>
       <c r="AN17" s="36">
         <v>5</v>
       </c>
-      <c r="AO17" s="37">
+      <c r="AO17" s="36">
         <v>5</v>
       </c>
-      <c r="AP17" s="25" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="AP17" s="37">
+        <v>5</v>
+      </c>
+      <c r="AQ17" s="25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>164</v>
       </c>
@@ -3817,7 +3894,7 @@
         <v>50</v>
       </c>
       <c r="P18" s="4" t="str">
-        <f t="shared" ref="P18" si="3">IF(COUNTIF(Q18:T18,"yes")&gt;0,"yes",IF(COUNTBLANK(Q18:T18)&gt;0,"","no"))</f>
+        <f t="shared" ref="P18" si="4">IF(COUNTIF(Q18:T18,"yes")&gt;0,"yes",IF(COUNTBLANK(Q18:T18)&gt;0,"","no"))</f>
         <v>no</v>
       </c>
       <c r="Q18" s="6" t="s">
@@ -3845,55 +3922,59 @@
         <v>67</v>
       </c>
       <c r="Y18" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="Z18" t="s">
-        <v>59</v>
+        <v>96</v>
+      </c>
+      <c r="Z18" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="AA18" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB18" t="s">
         <v>156</v>
       </c>
-      <c r="AC18" t="s">
+      <c r="AD18" t="s">
         <v>67</v>
       </c>
-      <c r="AD18" t="s">
+      <c r="AE18" t="s">
         <v>97</v>
       </c>
-      <c r="AE18" t="s">
+      <c r="AF18" t="s">
         <v>64</v>
       </c>
-      <c r="AF18" t="s">
+      <c r="AG18" t="s">
         <v>65</v>
       </c>
-      <c r="AG18" t="s">
+      <c r="AH18" t="s">
         <v>167</v>
       </c>
-      <c r="AH18" t="s">
+      <c r="AI18" t="s">
         <v>132</v>
       </c>
-      <c r="AI18" t="s">
+      <c r="AJ18" t="s">
         <v>66</v>
       </c>
-      <c r="AK18" s="35">
+      <c r="AL18" s="35">
         <v>2</v>
       </c>
-      <c r="AL18" s="36" t="s">
+      <c r="AM18" s="36" t="s">
         <v>166</v>
-      </c>
-      <c r="AM18" s="36">
-        <v>5</v>
       </c>
       <c r="AN18" s="36">
         <v>5</v>
       </c>
-      <c r="AO18" s="37">
+      <c r="AO18" s="36">
         <v>5</v>
       </c>
-      <c r="AP18" s="25" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="19" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="AP18" s="37">
+        <v>5</v>
+      </c>
+      <c r="AQ18" s="25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>169</v>
       </c>
@@ -3940,7 +4021,7 @@
         <v>50</v>
       </c>
       <c r="P19" s="4" t="str">
-        <f t="shared" ref="P19" si="4">IF(COUNTIF(Q19:T19,"yes")&gt;0,"yes",IF(COUNTBLANK(Q19:T19)&gt;0,"","no"))</f>
+        <f t="shared" ref="P19" si="5">IF(COUNTIF(Q19:T19,"yes")&gt;0,"yes",IF(COUNTBLANK(Q19:T19)&gt;0,"","no"))</f>
         <v>no</v>
       </c>
       <c r="Q19" s="6" t="s">
@@ -3970,595 +4051,742 @@
       <c r="Y19" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="Z19" t="s">
+      <c r="Z19" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AA19" t="s">
         <v>57</v>
       </c>
-      <c r="AA19" t="s">
+      <c r="AB19" t="s">
         <v>81</v>
       </c>
-      <c r="AB19" t="s">
+      <c r="AC19" t="s">
         <v>172</v>
       </c>
-      <c r="AC19" t="s">
+      <c r="AD19" t="s">
         <v>67</v>
       </c>
-      <c r="AD19" t="s">
+      <c r="AE19" t="s">
         <v>82</v>
       </c>
-      <c r="AE19" t="s">
+      <c r="AF19" t="s">
         <v>64</v>
       </c>
-      <c r="AF19" t="s">
+      <c r="AG19" t="s">
         <v>105</v>
       </c>
-      <c r="AG19" t="s">
+      <c r="AH19" t="s">
         <v>173</v>
       </c>
-      <c r="AH19" t="s">
+      <c r="AI19" t="s">
         <v>151</v>
       </c>
-      <c r="AI19" t="s">
+      <c r="AJ19" t="s">
         <v>98</v>
       </c>
-      <c r="AJ19" t="s">
+      <c r="AK19" t="s">
         <v>174</v>
       </c>
-      <c r="AK19" s="35">
+      <c r="AL19" s="35">
         <v>3</v>
       </c>
-      <c r="AL19" s="36" t="s">
+      <c r="AM19" s="36" t="s">
         <v>171</v>
-      </c>
-      <c r="AM19" s="36">
-        <v>5</v>
       </c>
       <c r="AN19" s="36">
         <v>5</v>
       </c>
-      <c r="AO19" s="37">
+      <c r="AO19" s="36">
         <v>5</v>
       </c>
-      <c r="AP19" s="25" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="AP19" s="37">
+        <v>5</v>
+      </c>
+      <c r="AQ19" s="25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A20" s="2"/>
       <c r="C20" s="40"/>
       <c r="J20" s="45"/>
       <c r="Y20" s="23"/>
-    </row>
-    <row r="21" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="Z20" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A21" s="2"/>
       <c r="Y21" s="23"/>
-    </row>
-    <row r="22" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="Z21" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A22" s="2"/>
       <c r="Y22" s="23"/>
-    </row>
-    <row r="23" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="Z22" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A23" s="2"/>
       <c r="Y23" s="23"/>
-    </row>
-    <row r="24" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="Z23" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A24" s="2"/>
       <c r="Y24" s="23"/>
-    </row>
-    <row r="25" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="Z24" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A25" s="2"/>
       <c r="Y25" s="23"/>
-    </row>
-    <row r="26" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="Z25" s="1"/>
+    </row>
+    <row r="26" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A26" s="2"/>
       <c r="Y26" s="23"/>
-      <c r="AG26" s="1"/>
+      <c r="Z26" s="1"/>
       <c r="AH26" s="1"/>
       <c r="AI26" s="1"/>
-    </row>
-    <row r="27" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="AJ26" s="1"/>
+    </row>
+    <row r="27" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A27" s="2"/>
       <c r="Y27" s="23"/>
-    </row>
-    <row r="28" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="Z27" s="1"/>
+    </row>
+    <row r="28" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A28" s="2"/>
       <c r="Y28" s="23"/>
-    </row>
-    <row r="29" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="Z28" s="1"/>
+    </row>
+    <row r="29" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A29" s="2"/>
       <c r="Y29" s="23"/>
-    </row>
-    <row r="30" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="Z29" s="1"/>
+    </row>
+    <row r="30" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A30" s="2"/>
       <c r="Y30" s="23"/>
-    </row>
-    <row r="31" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="Z30" s="1"/>
+    </row>
+    <row r="31" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A31" s="2"/>
       <c r="Y31" s="23"/>
-    </row>
-    <row r="32" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="Z31" s="1"/>
+    </row>
+    <row r="32" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A32" s="2"/>
       <c r="Y32" s="23"/>
-    </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z32" s="1"/>
+    </row>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A33" s="2"/>
       <c r="Y33" s="23"/>
-    </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z33" s="1"/>
+    </row>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A34" s="2"/>
       <c r="Y34" s="23"/>
-    </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z34" s="1"/>
+    </row>
+    <row r="35" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A35" s="2"/>
       <c r="Y35" s="23"/>
-    </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z35" s="1"/>
+    </row>
+    <row r="36" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A36" s="2"/>
       <c r="Y36" s="23"/>
-    </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z36" s="1"/>
+    </row>
+    <row r="37" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A37" s="2"/>
       <c r="Y37" s="23"/>
-    </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z37" s="1"/>
+    </row>
+    <row r="38" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A38" s="2"/>
       <c r="Y38" s="23"/>
-    </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z38" s="1"/>
+    </row>
+    <row r="39" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A39" s="2"/>
       <c r="Y39" s="23"/>
-    </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z39" s="1"/>
+    </row>
+    <row r="40" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A40" s="2"/>
       <c r="Y40" s="23"/>
-    </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z40" s="1"/>
+    </row>
+    <row r="41" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A41" s="2"/>
       <c r="Y41" s="23"/>
-    </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z41" s="1"/>
+    </row>
+    <row r="42" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A42" s="2"/>
       <c r="Y42" s="23"/>
-    </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z42" s="1"/>
+    </row>
+    <row r="43" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A43" s="2"/>
       <c r="Y43" s="23"/>
-    </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z43" s="1"/>
+    </row>
+    <row r="44" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A44" s="2"/>
       <c r="Y44" s="23"/>
-    </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z44" s="1"/>
+    </row>
+    <row r="45" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A45" s="2"/>
       <c r="Y45" s="23"/>
-    </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z45" s="1"/>
+    </row>
+    <row r="46" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A46" s="2"/>
       <c r="Y46" s="23"/>
-    </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z46" s="1"/>
+    </row>
+    <row r="47" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A47" s="2"/>
       <c r="Y47" s="23"/>
-    </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z47" s="1"/>
+    </row>
+    <row r="48" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A48" s="2"/>
       <c r="Y48" s="23"/>
-    </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z48" s="1"/>
+    </row>
+    <row r="49" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A49" s="2"/>
       <c r="Y49" s="23"/>
-    </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z49" s="1"/>
+    </row>
+    <row r="50" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A50" s="2"/>
       <c r="Y50" s="23"/>
-    </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z50" s="1"/>
+    </row>
+    <row r="51" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A51" s="2"/>
       <c r="Y51" s="23"/>
-    </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z51" s="1"/>
+    </row>
+    <row r="52" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A52" s="2"/>
     </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A53" s="2"/>
       <c r="Y53" s="23"/>
-    </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z53" s="1"/>
+    </row>
+    <row r="54" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A54" s="2"/>
       <c r="Y54" s="23"/>
-    </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z54" s="1"/>
+    </row>
+    <row r="55" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A55" s="2"/>
       <c r="Y55" s="23"/>
-    </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z55" s="1"/>
+    </row>
+    <row r="56" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A56" s="2"/>
       <c r="Y56" s="23"/>
-    </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z56" s="1"/>
+    </row>
+    <row r="57" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A57" s="2"/>
       <c r="Y57" s="23"/>
-    </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z57" s="1"/>
+    </row>
+    <row r="58" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A58" s="2"/>
       <c r="Y58" s="23"/>
-    </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z58" s="1"/>
+    </row>
+    <row r="59" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A59" s="2"/>
       <c r="Y59" s="23"/>
-    </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z59" s="1"/>
+    </row>
+    <row r="60" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A60" s="2"/>
       <c r="Y60" s="23"/>
-    </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z60" s="1"/>
+    </row>
+    <row r="61" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A61" s="2"/>
     </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A62" s="2"/>
       <c r="Y62" s="23"/>
-    </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z62" s="1"/>
+    </row>
+    <row r="63" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A63" s="2"/>
       <c r="Y63" s="23"/>
-    </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z63" s="1"/>
+    </row>
+    <row r="64" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A64" s="2"/>
       <c r="Y64" s="23"/>
-    </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z64" s="1"/>
+    </row>
+    <row r="65" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A65" s="2"/>
       <c r="Y65" s="23"/>
-    </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z65" s="1"/>
+    </row>
+    <row r="66" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A66" s="2"/>
       <c r="Y66" s="23"/>
-    </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z66" s="1"/>
+    </row>
+    <row r="67" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A67" s="2"/>
       <c r="Y67" s="23"/>
-    </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z67" s="1"/>
+    </row>
+    <row r="68" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A68" s="2"/>
       <c r="Y68" s="23"/>
-    </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z68" s="1"/>
+    </row>
+    <row r="69" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A69" s="2"/>
       <c r="Y69" s="23"/>
-    </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z69" s="1"/>
+    </row>
+    <row r="70" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A70" s="2"/>
       <c r="Y70" s="23"/>
-    </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z70" s="1"/>
+    </row>
+    <row r="71" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A71" s="2"/>
       <c r="Y71" s="23"/>
-    </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z71" s="1"/>
+    </row>
+    <row r="72" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A72" s="2"/>
       <c r="Y72" s="23"/>
-    </row>
-    <row r="73" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z72" s="1"/>
+    </row>
+    <row r="73" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A73" s="2"/>
       <c r="Y73" s="23"/>
-    </row>
-    <row r="74" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z73" s="1"/>
+    </row>
+    <row r="74" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A74" s="2"/>
       <c r="Y74" s="23"/>
-    </row>
-    <row r="75" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z74" s="1"/>
+    </row>
+    <row r="75" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A75" s="2"/>
       <c r="Y75" s="23"/>
-    </row>
-    <row r="76" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z75" s="1"/>
+    </row>
+    <row r="76" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A76" s="2"/>
     </row>
-    <row r="77" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A77" s="2"/>
       <c r="Y77" s="23"/>
-    </row>
-    <row r="78" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z77" s="1"/>
+    </row>
+    <row r="78" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A78" s="2"/>
       <c r="Y78" s="23"/>
-    </row>
-    <row r="79" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z78" s="1"/>
+    </row>
+    <row r="79" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A79" s="2"/>
       <c r="Y79" s="23"/>
-    </row>
-    <row r="80" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z79" s="1"/>
+    </row>
+    <row r="80" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A80" s="2"/>
       <c r="Y80" s="23"/>
-    </row>
-    <row r="81" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z80" s="1"/>
+    </row>
+    <row r="81" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A81" s="2"/>
       <c r="Y81" s="23"/>
-    </row>
-    <row r="82" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z81" s="1"/>
+    </row>
+    <row r="82" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A82" s="2"/>
       <c r="Y82" s="23"/>
-    </row>
-    <row r="83" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z82" s="1"/>
+    </row>
+    <row r="83" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A83" s="2"/>
       <c r="Y83" s="23"/>
-    </row>
-    <row r="84" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z83" s="1"/>
+    </row>
+    <row r="84" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A84" s="2"/>
       <c r="Y84" s="23"/>
-    </row>
-    <row r="85" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z84" s="1"/>
+    </row>
+    <row r="85" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A85" s="2"/>
       <c r="Y85" s="23"/>
-    </row>
-    <row r="86" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z85" s="1"/>
+    </row>
+    <row r="86" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A86" s="2"/>
       <c r="Y86" s="23"/>
-    </row>
-    <row r="87" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z86" s="1"/>
+    </row>
+    <row r="87" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A87" s="2"/>
       <c r="Y87" s="23"/>
-    </row>
-    <row r="88" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z87" s="1"/>
+    </row>
+    <row r="88" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A88" s="2"/>
       <c r="Y88" s="23"/>
-    </row>
-    <row r="89" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z88" s="1"/>
+    </row>
+    <row r="89" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A89" s="2"/>
       <c r="Y89" s="23"/>
-    </row>
-    <row r="90" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z89" s="1"/>
+    </row>
+    <row r="90" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A90" s="2"/>
       <c r="Y90" s="23"/>
-    </row>
-    <row r="91" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z90" s="1"/>
+    </row>
+    <row r="91" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A91" s="2"/>
       <c r="Y91" s="23"/>
-    </row>
-    <row r="92" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z91" s="1"/>
+    </row>
+    <row r="92" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A92" s="2"/>
       <c r="Y92" s="23"/>
-    </row>
-    <row r="93" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z92" s="1"/>
+    </row>
+    <row r="93" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A93" s="2"/>
       <c r="Y93" s="23"/>
-    </row>
-    <row r="94" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z93" s="1"/>
+    </row>
+    <row r="94" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A94" s="2"/>
       <c r="Y94" s="23"/>
-    </row>
-    <row r="95" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z94" s="1"/>
+    </row>
+    <row r="95" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A95" s="2"/>
       <c r="Y95" s="23"/>
-    </row>
-    <row r="96" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z95" s="1"/>
+    </row>
+    <row r="96" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A96" s="2"/>
       <c r="Y96" s="23"/>
-    </row>
-    <row r="97" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z96" s="1"/>
+    </row>
+    <row r="97" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A97" s="2"/>
       <c r="Y97" s="23"/>
-    </row>
-    <row r="98" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z97" s="1"/>
+    </row>
+    <row r="98" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A98" s="2"/>
       <c r="Y98" s="23"/>
-    </row>
-    <row r="99" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z98" s="1"/>
+    </row>
+    <row r="99" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A99" s="2"/>
       <c r="Y99" s="23"/>
-    </row>
-    <row r="100" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z99" s="1"/>
+    </row>
+    <row r="100" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A100" s="2"/>
       <c r="Y100" s="23"/>
-    </row>
-    <row r="101" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z100" s="1"/>
+    </row>
+    <row r="101" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A101" s="2"/>
     </row>
-    <row r="102" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A102" s="2"/>
       <c r="Y102" s="23"/>
-    </row>
-    <row r="103" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z102" s="1"/>
+    </row>
+    <row r="103" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A103" s="2"/>
       <c r="Y103" s="23"/>
-    </row>
-    <row r="104" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z103" s="1"/>
+    </row>
+    <row r="104" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A104" s="2"/>
       <c r="Y104" s="23"/>
-    </row>
-    <row r="105" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z104" s="1"/>
+    </row>
+    <row r="105" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A105" s="2"/>
       <c r="Y105" s="23"/>
-    </row>
-    <row r="106" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z105" s="1"/>
+    </row>
+    <row r="106" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A106" s="2"/>
       <c r="Y106" s="23"/>
-    </row>
-    <row r="107" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z106" s="1"/>
+    </row>
+    <row r="107" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A107" s="2"/>
       <c r="Y107" s="23"/>
-    </row>
-    <row r="108" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z107" s="1"/>
+    </row>
+    <row r="108" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A108" s="2"/>
       <c r="Y108" s="23"/>
-    </row>
-    <row r="109" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z108" s="1"/>
+    </row>
+    <row r="109" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A109" s="2"/>
       <c r="Y109" s="23"/>
-    </row>
-    <row r="110" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z109" s="1"/>
+    </row>
+    <row r="110" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A110" s="2"/>
       <c r="Y110" s="23"/>
-    </row>
-    <row r="111" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z110" s="1"/>
+    </row>
+    <row r="111" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A111" s="2"/>
       <c r="Y111" s="23"/>
-    </row>
-    <row r="112" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z111" s="1"/>
+    </row>
+    <row r="112" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A112" s="2"/>
       <c r="Y112" s="23"/>
-    </row>
-    <row r="113" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z112" s="1"/>
+    </row>
+    <row r="113" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A113" s="2"/>
       <c r="Y113" s="23"/>
-    </row>
-    <row r="114" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z113" s="1"/>
+    </row>
+    <row r="114" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A114" s="2"/>
       <c r="Y114" s="23"/>
-    </row>
-    <row r="115" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z114" s="1"/>
+    </row>
+    <row r="115" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A115" s="2"/>
       <c r="Y115" s="23"/>
-    </row>
-    <row r="116" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z115" s="1"/>
+    </row>
+    <row r="116" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A116" s="2"/>
       <c r="Y116" s="23"/>
-    </row>
-    <row r="117" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z116" s="1"/>
+    </row>
+    <row r="117" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A117" s="2"/>
       <c r="Y117" s="23"/>
-    </row>
-    <row r="118" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z117" s="1"/>
+    </row>
+    <row r="118" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A118" s="2"/>
       <c r="Y118" s="23"/>
-    </row>
-    <row r="119" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z118" s="1"/>
+    </row>
+    <row r="119" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A119" s="2"/>
       <c r="Y119" s="23"/>
-    </row>
-    <row r="120" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z119" s="1"/>
+    </row>
+    <row r="120" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A120" s="2"/>
       <c r="Y120" s="23"/>
-    </row>
-    <row r="121" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z120" s="1"/>
+    </row>
+    <row r="121" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A121" s="2"/>
       <c r="Y121" s="23"/>
-    </row>
-    <row r="122" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z121" s="1"/>
+    </row>
+    <row r="122" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A122" s="2"/>
       <c r="Y122" s="23"/>
-    </row>
-    <row r="123" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z122" s="1"/>
+    </row>
+    <row r="123" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A123" s="2"/>
       <c r="Y123" s="23"/>
-    </row>
-    <row r="124" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z123" s="1"/>
+    </row>
+    <row r="124" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A124" s="2"/>
       <c r="Y124" s="23"/>
-    </row>
-    <row r="125" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z124" s="1"/>
+    </row>
+    <row r="125" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A125" s="2"/>
       <c r="Y125" s="23"/>
-    </row>
-    <row r="126" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z125" s="1"/>
+    </row>
+    <row r="126" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A126" s="2"/>
     </row>
-    <row r="127" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A127" s="2"/>
       <c r="Y127" s="23"/>
-    </row>
-    <row r="128" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z127" s="1"/>
+    </row>
+    <row r="128" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A128" s="2"/>
       <c r="Y128" s="23"/>
-    </row>
-    <row r="129" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z128" s="1"/>
+    </row>
+    <row r="129" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A129" s="2"/>
       <c r="Y129" s="23"/>
-    </row>
-    <row r="130" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z129" s="1"/>
+    </row>
+    <row r="130" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A130" s="2"/>
       <c r="Y130" s="23"/>
-    </row>
-    <row r="131" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z130" s="1"/>
+    </row>
+    <row r="131" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A131" s="2"/>
       <c r="Y131" s="23"/>
-    </row>
-    <row r="132" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z131" s="1"/>
+    </row>
+    <row r="132" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A132" s="2"/>
       <c r="Y132" s="23"/>
-    </row>
-    <row r="133" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z132" s="1"/>
+    </row>
+    <row r="133" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A133" s="2"/>
       <c r="Y133" s="23"/>
-    </row>
-    <row r="134" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z133" s="1"/>
+    </row>
+    <row r="134" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A134" s="2"/>
       <c r="Y134" s="23"/>
-    </row>
-    <row r="135" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z134" s="1"/>
+    </row>
+    <row r="135" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A135" s="2"/>
       <c r="Y135" s="23"/>
-    </row>
-    <row r="136" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z135" s="1"/>
+    </row>
+    <row r="136" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A136" s="2"/>
       <c r="Y136" s="23"/>
-    </row>
-    <row r="137" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z136" s="1"/>
+    </row>
+    <row r="137" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A137" s="2"/>
     </row>
-    <row r="138" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A138" s="2"/>
       <c r="Y138" s="23"/>
-    </row>
-    <row r="139" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z138" s="1"/>
+    </row>
+    <row r="139" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A139" s="2"/>
       <c r="Y139" s="23"/>
-    </row>
-    <row r="140" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z139" s="1"/>
+    </row>
+    <row r="140" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A140" s="2"/>
       <c r="Y140" s="23"/>
-    </row>
-    <row r="141" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z140" s="1"/>
+    </row>
+    <row r="141" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A141" s="2"/>
       <c r="Y141" s="23"/>
-    </row>
-    <row r="142" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z141" s="1"/>
+    </row>
+    <row r="142" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A142" s="2"/>
       <c r="Y142" s="23"/>
-    </row>
-    <row r="143" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z142" s="1"/>
+    </row>
+    <row r="143" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A143" s="2"/>
       <c r="Y143" s="23"/>
-    </row>
-    <row r="144" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z143" s="1"/>
+    </row>
+    <row r="144" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A144" s="2"/>
       <c r="Y144" s="23"/>
-    </row>
-    <row r="145" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z144" s="1"/>
+    </row>
+    <row r="145" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A145" s="2"/>
       <c r="Y145" s="23"/>
-    </row>
-    <row r="146" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z145" s="1"/>
+    </row>
+    <row r="146" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A146" s="2"/>
       <c r="Y146" s="23"/>
-    </row>
-    <row r="147" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z146" s="1"/>
+    </row>
+    <row r="147" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A147" s="2"/>
       <c r="Y147" s="23"/>
-    </row>
-    <row r="148" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z147" s="1"/>
+    </row>
+    <row r="148" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A148" s="2"/>
       <c r="Y148" s="23"/>
-    </row>
-    <row r="149" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z148" s="1"/>
+    </row>
+    <row r="149" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A149" s="2"/>
       <c r="Y149" s="23"/>
-    </row>
-    <row r="150" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z149" s="1"/>
+    </row>
+    <row r="150" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A150" s="2"/>
     </row>
-    <row r="151" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A151" s="2"/>
       <c r="Y151" s="23"/>
-    </row>
-    <row r="152" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z151" s="1"/>
+    </row>
+    <row r="152" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A152" s="2"/>
       <c r="Y152" s="23"/>
-    </row>
-    <row r="153" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z152" s="1"/>
+    </row>
+    <row r="153" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A153" s="2"/>
       <c r="Y153" s="23"/>
-    </row>
-    <row r="154" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z153" s="1"/>
+    </row>
+    <row r="154" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A154" s="2"/>
       <c r="Y154" s="23"/>
+      <c r="Z154" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="P2:P15 P20:P29">
@@ -4595,8 +4823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5E501FD-8D50-44D6-A0B2-1A8A34E60684}">
   <dimension ref="A1:Z14"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="82" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7:M7"/>
+    <sheetView zoomScale="82" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>